<commit_message>
xóa & tim k
</commit_message>
<xml_diff>
--- a/TinhNQ/tailieu/Huong dan created website.xlsx
+++ b/TinhNQ/tailieu/Huong dan created website.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>quản lý backend</t>
   </si>
@@ -163,6 +163,72 @@
   </si>
   <si>
     <t>và gọi đến method common select_array trong file csdl.php</t>
+  </si>
+  <si>
+    <t>Chức năng xóa</t>
+  </si>
+  <si>
+    <t>phần 1 :</t>
+  </si>
+  <si>
+    <t>Phần 2 :</t>
+  </si>
+  <si>
+    <t>gán text xóa vào link</t>
+  </si>
+  <si>
+    <t>nhacungcap_list.php?xoa=true&amp;MaNhaCungCap=6</t>
+  </si>
+  <si>
+    <t>kiểm tra có phải biến xóa = true</t>
+  </si>
+  <si>
+    <t>và mã nhà cung cấp có giá trị k?</t>
+  </si>
+  <si>
+    <t>Viết câu lệnh sql xóa theo mã nhà cung cấp</t>
+  </si>
+  <si>
+    <t>thực hiện xoa</t>
+  </si>
+  <si>
+    <t>Xóa thành công thì hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>add đoạn js xử lý : hỏi trước khi xóa</t>
+  </si>
+  <si>
+    <t>chức năng tìm kiếm tên nhà cung cấp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phần HTML </t>
+  </si>
+  <si>
+    <t>thêm 1 dòng</t>
+  </si>
+  <si>
+    <t>chứa label, textbox, button</t>
+  </si>
+  <si>
+    <t>và form</t>
+  </si>
+  <si>
+    <t>nhacungcap_list</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Phần PHP</t>
+  </si>
+  <si>
+    <t>kiểm tra điều kiện search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add điều kiện where sử dụng like </t>
+  </si>
+  <si>
+    <t>nối chuỗi vào câu sql</t>
   </si>
 </sst>
 </file>
@@ -521,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M47"/>
+  <dimension ref="B2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" topLeftCell="B57" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +840,128 @@
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>62</v>
+      </c>
+      <c r="H60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>